<commit_message>
add markdown.html file from createdom.py script. edit default.html to point to a script that doesnt build the dom anymore
</commit_message>
<xml_diff>
--- a/js/data/data.xlsx
+++ b/js/data/data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25516"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="2980" yWindow="320" windowWidth="34100" windowHeight="19660" tabRatio="500"/>
+    <workbookView xWindow="10260" yWindow="120" windowWidth="39600" windowHeight="26020" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Questions" sheetId="1" r:id="rId1"/>
@@ -56,9 +56,6 @@
     <t>Result Text</t>
   </si>
   <si>
-    <t>Test your Power Grid IQ</t>
-  </si>
-  <si>
     <t>Do you know your synchrophasors from your micro grids? Test your knowledge of the electric grid with our grid IQ test.</t>
   </si>
   <si>
@@ -309,6 +306,9 @@
   </si>
   <si>
     <t>Neither</t>
+  </si>
+  <si>
+    <t>Test your &lt;span class="green-text"&gt;Power Grid&lt;/span&gt; IQ</t>
   </si>
 </sst>
 </file>
@@ -717,7 +717,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+    <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
@@ -753,255 +753,255 @@
     </row>
     <row r="2" spans="1:7" ht="60">
       <c r="A2" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B2" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="C2" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="D2" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="E2" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="G2" s="3" t="s">
         <v>22</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>94</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="G2" s="3" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="30">
       <c r="A3" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B3" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="C3" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="D3" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="E3" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="E3" s="3" t="s">
+      <c r="F3" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="G3" s="3" t="s">
         <v>28</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>84</v>
-      </c>
-      <c r="G3" s="3" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="4" spans="1:7">
       <c r="A4" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B4" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="C4" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="D4" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="E4" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="E4" s="3" t="s">
+      <c r="F4" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="G4" s="3" t="s">
         <v>34</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>85</v>
-      </c>
-      <c r="G4" s="3" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="60">
       <c r="A5" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="B5" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="C5" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="D5" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="D5" s="3" t="s">
+      <c r="E5" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="G5" s="3" t="s">
         <v>39</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>95</v>
-      </c>
-      <c r="F5" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="G5" s="3" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="30">
       <c r="A6" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="B6" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="C6" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="D6" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="D6" s="3" t="s">
+      <c r="E6" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="E6" s="3" t="s">
+      <c r="F6" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="G6" s="3" t="s">
         <v>45</v>
-      </c>
-      <c r="F6" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="G6" s="3" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="45">
       <c r="A7" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="B7" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="C7" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="C7" s="3" t="s">
+      <c r="D7" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="D7" s="3" t="s">
+      <c r="E7" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="E7" s="3" t="s">
+      <c r="F7" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="G7" s="3" t="s">
         <v>51</v>
-      </c>
-      <c r="F7" s="3" t="s">
-        <v>88</v>
-      </c>
-      <c r="G7" s="3" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="30">
       <c r="A8" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="B8" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="C8" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="C8" s="3" t="s">
+      <c r="D8" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="D8" s="3" t="s">
+      <c r="E8" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="E8" s="3" t="s">
+      <c r="F8" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="G8" s="3" t="s">
         <v>57</v>
-      </c>
-      <c r="F8" s="3" t="s">
-        <v>89</v>
-      </c>
-      <c r="G8" s="3" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="30">
       <c r="A9" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="B9" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="B9" s="4" t="s">
+      <c r="C9" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="C9" s="3" t="s">
+      <c r="D9" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="D9" s="3" t="s">
+      <c r="E9" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="E9" s="3" t="s">
+      <c r="F9" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="G9" s="3" t="s">
         <v>63</v>
-      </c>
-      <c r="F9" s="3" t="s">
-        <v>90</v>
-      </c>
-      <c r="G9" s="3" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="30">
       <c r="A10" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="B10" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="B10" s="3" t="s">
+      <c r="C10" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="C10" s="3" t="s">
+      <c r="D10" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="D10" s="3" t="s">
+      <c r="E10" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="E10" s="3" t="s">
+      <c r="F10" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="G10" s="3" t="s">
         <v>69</v>
-      </c>
-      <c r="F10" s="3" t="s">
-        <v>91</v>
-      </c>
-      <c r="G10" s="3" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="30">
       <c r="A11" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="B11" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="B11" s="3" t="s">
+      <c r="C11" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="C11" s="3" t="s">
+      <c r="D11" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="D11" s="3" t="s">
+      <c r="E11" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="E11" s="3" t="s">
+      <c r="F11" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="G11" s="3" t="s">
         <v>75</v>
-      </c>
-      <c r="F11" s="3" t="s">
-        <v>92</v>
-      </c>
-      <c r="G11" s="3" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="30">
       <c r="A12" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="B12" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="B12" s="3" t="s">
+      <c r="C12" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="C12" s="3" t="s">
+      <c r="D12" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="D12" s="3" t="s">
+      <c r="E12" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="E12" s="3" t="s">
+      <c r="F12" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="G12" s="3" t="s">
         <v>81</v>
-      </c>
-      <c r="F12" s="3" t="s">
-        <v>93</v>
-      </c>
-      <c r="G12" s="3" t="s">
-        <v>82</v>
       </c>
     </row>
   </sheetData>
@@ -1019,14 +1019,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="21.5" customWidth="1"/>
-    <col min="2" max="2" width="26.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="82.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -1037,12 +1037,12 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="75">
+    <row r="2" spans="1:2" ht="30">
       <c r="A2" t="s">
+        <v>95</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>11</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>12</v>
       </c>
     </row>
   </sheetData>
@@ -1060,14 +1060,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C9"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="2" width="18.83203125" customWidth="1"/>
-    <col min="3" max="3" width="18.6640625" customWidth="1"/>
+    <col min="3" max="3" width="122.5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -1077,16 +1077,16 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" t="s">
         <v>13</v>
-      </c>
-      <c r="B2" t="s">
-        <v>14</v>
       </c>
       <c r="C2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="120">
+    <row r="3" spans="1:3">
       <c r="A3" s="2">
         <v>0</v>
       </c>
@@ -1094,10 +1094,10 @@
         <v>2</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" ht="90">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -1105,10 +1105,10 @@
         <v>5</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" ht="135">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="30">
       <c r="A5" s="2">
         <v>6</v>
       </c>
@@ -1116,10 +1116,10 @@
         <v>8</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" ht="120">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
       <c r="A6" s="2">
         <v>9</v>
       </c>
@@ -1127,7 +1127,7 @@
         <v>11</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="10" customHeight="1"/>

</xml_diff>